<commit_message>
make room for core grant dept
</commit_message>
<xml_diff>
--- a/site/application/backend/app-public/View/Layouts/mac-template.xlsx
+++ b/site/application/backend/app-public/View/Layouts/mac-template.xlsx
@@ -146,8 +146,8 @@
     <numFmt numFmtId="165" formatCode="d/m/yy"/>
     <numFmt numFmtId="166" formatCode="dd/MM/yyyy"/>
     <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="168" formatCode="[$£]#,##0"/>
-    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0;\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="168" formatCode="&quot;£&quot;#,##0;\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="169" formatCode="[$£]#,##0"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -160,13 +160,13 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial Narrow"/>
     </font>
+    <font/>
     <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF205867"/>
       <name val="Trebuchet MS"/>
     </font>
-    <font/>
     <font>
       <sz val="12.0"/>
       <color rgb="FF632423"/>
@@ -264,12 +264,6 @@
       <name val="Trebuchet MS"/>
     </font>
     <font>
-      <b/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color rgb="FF1F497D"/>
       <name val="Trebuchet MS"/>
@@ -277,6 +271,12 @@
     <font>
       <sz val="11.0"/>
       <name val="Trebuchet MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="12.0"/>
@@ -351,14 +351,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD6E3BC"/>
-        <bgColor rgb="FFD6E3BC"/>
+        <fgColor rgb="FFB2A1C7"/>
+        <bgColor rgb="FFB2A1C7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB2A1C7"/>
-        <bgColor rgb="FFB2A1C7"/>
+        <fgColor rgb="FFD6E3BC"/>
+        <bgColor rgb="FFD6E3BC"/>
       </patternFill>
     </fill>
     <fill>
@@ -392,18 +392,6 @@
       <bottom/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -412,7 +400,9 @@
       <bottom/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -428,6 +418,16 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -504,214 +504,214 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="3" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="4" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="0" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="5" fontId="13" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="2" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="15" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="15" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="3" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="16" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="6" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="7" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="7" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="8" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="9" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="9" fontId="14" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="8" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="9" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="19" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="9" fontId="19" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="10" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="10" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="19" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="10" fontId="21" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="10" fontId="21" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="10" fontId="20" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="10" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="10" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="9" fontId="19" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="9" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="8" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="10" fontId="20" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="11" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="10" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="11" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="10" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="22" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="22" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="11" fontId="20" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="23" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="11" fontId="20" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="23" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="23" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="4" fontId="24" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="24" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="4" fontId="23" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="4" fontId="23" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="24" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="4" fontId="24" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="4" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="22" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="3" fillId="5" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="26" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="27" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="24" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="19" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="26" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="26" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="26" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="11" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="27" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="28" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="0" fontId="28" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="19" numFmtId="168" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="4" fontId="19" numFmtId="169" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="4" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="4" fillId="4" fontId="19" numFmtId="10" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -744,47 +744,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="8" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="6"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="7"/>
       <c r="N1" s="11"/>
     </row>
     <row r="2" ht="34.5" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="6"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="6"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="7"/>
       <c r="K2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="6"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="11"/>
     </row>
     <row r="3" ht="30.75" customHeight="1">
@@ -800,18 +800,18 @@
       <c r="D3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="32" t="s">
+      <c r="J3" s="31" t="s">
         <v>25</v>
       </c>
       <c r="K3" s="33" t="s">
@@ -826,147 +826,147 @@
       <c r="N3" s="11"/>
     </row>
     <row r="4">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="37"/>
       <c r="C4" s="37"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="47"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="45"/>
       <c r="N4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="48"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="58"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="55"/>
       <c r="N5" s="11"/>
     </row>
     <row r="6">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="58"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+      <c r="M6" s="55"/>
       <c r="N6" s="11"/>
     </row>
     <row r="7">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="58"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="55"/>
       <c r="N7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="60"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="52"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="56"/>
-      <c r="L8" s="56"/>
-      <c r="M8" s="58"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="55"/>
       <c r="N8" s="11"/>
     </row>
     <row r="9">
-      <c r="A9" s="60"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="56"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="58"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="55"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="58"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="55"/>
       <c r="N10" s="11"/>
     </row>
     <row r="11">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="58"/>
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="55"/>
       <c r="N11" s="11"/>
     </row>
     <row r="12">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="55"/>
       <c r="N12" s="11"/>
     </row>
     <row r="13">
@@ -1148,32 +1148,32 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="5" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="10"/>
     </row>
     <row r="2">
       <c r="A2" s="12"/>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="10"/>
@@ -1182,15 +1182,15 @@
       <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
@@ -1208,7 +1208,7 @@
       <c r="E4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="23" t="s">
         <v>18</v>
       </c>
@@ -1224,55 +1224,55 @@
     </row>
     <row r="5">
       <c r="A5" s="29"/>
-      <c r="B5" s="31"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
     </row>
     <row r="6">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
     </row>
     <row r="7">
-      <c r="A7" s="51"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
     </row>
     <row r="8" ht="29.25" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" s="61" t="s">
@@ -1322,13 +1322,13 @@
       <c r="A11" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7"/>
       <c r="I11" s="70"/>
       <c r="J11" s="71"/>
     </row>
@@ -1336,13 +1336,13 @@
       <c r="A12" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="72"/>
       <c r="J12" s="72"/>
     </row>
@@ -1350,25 +1350,25 @@
       <c r="A13" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="43"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="46"/>
       <c r="I13" s="74"/>
       <c r="J13" s="74"/>
     </row>
     <row r="14">
-      <c r="A14" s="51"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="53"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="55"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="58"/>
       <c r="I14" s="75"/>
       <c r="J14" s="75"/>
     </row>
@@ -1379,14 +1379,14 @@
       <c r="B15" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16">
       <c r="B16" s="78"/>

</xml_diff>